<commit_message>
Updated boms and gerbers for Brunei
</commit_message>
<xml_diff>
--- a/EasyTelemetry/BMS_BOM.xlsx
+++ b/EasyTelemetry/BMS_BOM.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30405189-E670-4F0E-AF0F-450ECE524EFE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43C5AD5C-3198-49AA-9322-FC9F800B2978}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22257" windowHeight="12649" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="57">
   <si>
     <t>Digikey part</t>
   </si>
@@ -60,9 +60,6 @@
     <t>1uF</t>
   </si>
   <si>
-    <t>490-8311-1-ND</t>
-  </si>
-  <si>
     <t>10uF</t>
   </si>
   <si>
@@ -102,15 +99,9 @@
     <t>160-1456-1-ND</t>
   </si>
   <si>
-    <t>A114893-ND</t>
-  </si>
-  <si>
     <t>Val-U-Lok</t>
   </si>
   <si>
-    <t>2 pin</t>
-  </si>
-  <si>
     <t>A30603-ND</t>
   </si>
   <si>
@@ -123,9 +114,6 @@
     <t>1276-1068-1-ND</t>
   </si>
   <si>
-    <t>1k</t>
-  </si>
-  <si>
     <t>Capacitor</t>
   </si>
   <si>
@@ -184,6 +172,30 @@
   </si>
   <si>
     <t>1470-4531-ND</t>
+  </si>
+  <si>
+    <t>1276-2405-1-ND</t>
+  </si>
+  <si>
+    <t>47k</t>
+  </si>
+  <si>
+    <t>2.2k</t>
+  </si>
+  <si>
+    <t>1276-1931-1-ND</t>
+  </si>
+  <si>
+    <t>RMCF0603JT100RCT-ND</t>
+  </si>
+  <si>
+    <t>RMCF0603JT2K20CT-ND</t>
+  </si>
+  <si>
+    <t>RMCF0603JT10R0CT-ND</t>
+  </si>
+  <si>
+    <t>P20162CT-ND</t>
   </si>
 </sst>
 </file>
@@ -558,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -588,14 +600,14 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="I1" s="2">
-        <f>SUM(F2:F95)</f>
-        <v>58.42</v>
+        <f>SUM(F2:F94)</f>
+        <v>42.33</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -603,10 +615,10 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D2">
         <v>2.88</v>
@@ -621,13 +633,13 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3">
         <v>8</v>
@@ -636,19 +648,19 @@
         <v>1</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F23" si="0">E3*D3</f>
+        <f t="shared" ref="F3:F22" si="0">E3*D3</f>
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D4">
         <v>0.71</v>
@@ -663,13 +675,13 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D5">
         <v>0.6</v>
@@ -684,7 +696,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
@@ -696,22 +708,22 @@
         <v>0.17</v>
       </c>
       <c r="E6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
-        <v>0.68</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7">
         <v>0.14000000000000001</v>
@@ -726,13 +738,13 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
         <v>22</v>
-      </c>
-      <c r="C8" t="s">
-        <v>23</v>
       </c>
       <c r="D8">
         <v>0.34</v>
@@ -747,13 +759,13 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" t="s">
         <v>35</v>
-      </c>
-      <c r="C9" t="s">
-        <v>39</v>
       </c>
       <c r="D9">
         <v>0.5</v>
@@ -774,10 +786,10 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
         <v>16</v>
-      </c>
-      <c r="B11" t="s">
-        <v>17</v>
       </c>
       <c r="D11">
         <v>22.5</v>
@@ -792,10 +804,10 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
         <v>18</v>
-      </c>
-      <c r="B12" t="s">
-        <v>19</v>
       </c>
       <c r="D12">
         <v>3.95</v>
@@ -813,91 +825,100 @@
         <v>25</v>
       </c>
       <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
         <v>26</v>
       </c>
-      <c r="C14" t="s">
-        <v>27</v>
-      </c>
       <c r="D14">
-        <v>0.46</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="E14">
         <v>2</v>
       </c>
       <c r="F14">
         <f t="shared" si="0"/>
-        <v>0.92</v>
+        <v>1.1200000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16">
+        <v>100</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" t="s">
         <v>29</v>
       </c>
-      <c r="D15">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="E15">
-        <v>2</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="0"/>
-        <v>1.1200000000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="F16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>30</v>
-      </c>
-      <c r="C17">
-        <v>100</v>
       </c>
       <c r="E17">
         <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>55</v>
+      </c>
       <c r="B18" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" t="s">
-        <v>34</v>
+        <v>27</v>
+      </c>
+      <c r="C18" s="3">
+        <v>10</v>
       </c>
       <c r="E18">
         <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>54</v>
+      </c>
       <c r="B19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" s="3">
-        <v>10</v>
+        <v>27</v>
+      </c>
+      <c r="C19" t="s">
+        <v>51</v>
       </c>
       <c r="E19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
-        <v>30</v>
-      </c>
-      <c r="C20" t="s">
-        <v>32</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -907,70 +928,58 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" t="s">
+        <v>36</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
       <c r="F22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>41</v>
+      <c r="A23" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="E23">
         <v>1</v>
       </c>
-      <c r="F23">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B24" t="s">
-        <v>43</v>
-      </c>
-      <c r="D24">
-        <v>9</v>
-      </c>
-      <c r="E24">
-        <v>1</v>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B26" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B27" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>48</v>
-      </c>
-      <c r="B28" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A24" r:id="rId1" xr:uid="{7D360ED6-E210-44AD-84FE-68F0D27F2530}"/>
+    <hyperlink ref="A23" r:id="rId1" xr:uid="{7D360ED6-E210-44AD-84FE-68F0D27F2530}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="1200" r:id="rId2"/>

</xml_diff>